<commit_message>
Fix PRD pricing + remove founder salaries from forecast
## Pricing Alignment
- Technical PRD B2C pricing now matches Business PRD
- AI Interview Add-on: R500 → R1,250/role
- Added per-role pricing philosophy to Technical PRD

## Forecast Updates
- Full-Stack Developer: R82k → R80k
- Removed founder salaries (Simon & Shay)
- Monthly burn: R487k → R344k
- Break-even: Month 18 → Month 16
- Total funding: R5.5M → R3.8M

## Excel Updated
- HIREINBOX_18_Month_Forecast.xlsx reflects new figures

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/HIREINBOX_18_Month_Forecast.xlsx
+++ b/HIREINBOX_18_Month_Forecast.xlsx
@@ -557,7 +557,7 @@
       </c>
       <c r="B9" s="5" t="inlineStr">
         <is>
-          <t>R 404,000</t>
+          <t>R 344,000</t>
         </is>
       </c>
     </row>
@@ -1300,7 +1300,6 @@
         </is>
       </c>
     </row>
-    <row r="2"/>
     <row r="3">
       <c r="A3" s="6" t="inlineStr">
         <is>
@@ -1574,7 +1573,6 @@
         </is>
       </c>
     </row>
-    <row r="2"/>
     <row r="3">
       <c r="A3" s="6" t="inlineStr">
         <is>
@@ -1726,7 +1724,6 @@
         </is>
       </c>
     </row>
-    <row r="2"/>
     <row r="3">
       <c r="A3" s="6" t="inlineStr">
         <is>
@@ -1779,7 +1776,7 @@
       </c>
       <c r="B5" s="5" t="inlineStr">
         <is>
-          <t>R 60,000</t>
+          <t>R 80,000</t>
         </is>
       </c>
       <c r="C5" s="5" t="inlineStr">
@@ -1816,50 +1813,17 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="5" t="inlineStr">
-        <is>
-          <t>CEO (Simon Rubin)</t>
-        </is>
-      </c>
-      <c r="B7" s="5" t="inlineStr">
-        <is>
-          <t>R 40,000</t>
-        </is>
-      </c>
-      <c r="C7" s="5" t="inlineStr">
-        <is>
-          <t>1 Jul 2026</t>
-        </is>
-      </c>
-      <c r="D7" s="5" t="inlineStr">
-        <is>
-          <t>Below market, founder</t>
-        </is>
-      </c>
+      <c r="A7" s="5" t="n"/>
+      <c r="B7" s="5" t="n"/>
+      <c r="C7" s="5" t="n"/>
+      <c r="D7" s="5" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="5" t="inlineStr">
-        <is>
-          <t>Co-CEO (Shay Sinbeti)</t>
-        </is>
-      </c>
-      <c r="B8" s="5" t="inlineStr">
-        <is>
-          <t>R 40,000</t>
-        </is>
-      </c>
-      <c r="C8" s="5" t="inlineStr">
-        <is>
-          <t>1 Jul 2026</t>
-        </is>
-      </c>
-      <c r="D8" s="5" t="inlineStr">
-        <is>
-          <t>Below market, founder</t>
-        </is>
-      </c>
-    </row>
-    <row r="9"/>
+      <c r="A8" s="5" t="n"/>
+      <c r="B8" s="5" t="n"/>
+      <c r="C8" s="5" t="n"/>
+      <c r="D8" s="5" t="n"/>
+    </row>
     <row r="10">
       <c r="A10" s="10" t="inlineStr">
         <is>
@@ -1898,7 +1862,6 @@
         </is>
       </c>
     </row>
-    <row r="2"/>
     <row r="3">
       <c r="A3" s="6" t="inlineStr">
         <is>
@@ -1943,7 +1906,7 @@
         </is>
       </c>
       <c r="C5" s="11" t="n">
-        <v>60000</v>
+        <v>80000</v>
       </c>
     </row>
     <row r="6">
@@ -1962,34 +1925,14 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="5" t="inlineStr">
-        <is>
-          <t>Salaries</t>
-        </is>
-      </c>
-      <c r="B7" s="5" t="inlineStr">
-        <is>
-          <t>CEO (from Month 6)</t>
-        </is>
-      </c>
-      <c r="C7" s="11" t="n">
-        <v>40000</v>
-      </c>
+      <c r="A7" s="5" t="n"/>
+      <c r="B7" s="5" t="n"/>
+      <c r="C7" s="11" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="5" t="inlineStr">
-        <is>
-          <t>Salaries</t>
-        </is>
-      </c>
-      <c r="B8" s="5" t="inlineStr">
-        <is>
-          <t>Co-CEO (from Month 6)</t>
-        </is>
-      </c>
-      <c r="C8" s="11" t="n">
-        <v>40000</v>
-      </c>
+      <c r="A8" s="5" t="n"/>
+      <c r="B8" s="5" t="n"/>
+      <c r="C8" s="11" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="5" t="inlineStr">
@@ -2148,7 +2091,7 @@
         </is>
       </c>
       <c r="C19" s="13" t="n">
-        <v>404000</v>
+        <v>344000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>